<commit_message>
added SJM batch launcher
</commit_message>
<xml_diff>
--- a/udf-sas_job_manager.xlsx
+++ b/udf-sas_job_manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\sp-sas-job-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94E810A-FA2D-42D4-BF37-62F268A35A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126B164E-4838-4428-91B1-2AA4584253E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{7B78E075-C15E-42D8-990D-4107510A5C4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7B78E075-C15E-42D8-990D-4107510A5C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Template_History" sheetId="7" r:id="rId1"/>
@@ -648,9 +648,6 @@
     <t>Test Summary:</t>
   </si>
   <si>
-    <t>Unit Tests</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -915,6 +912,9 @@
   </si>
   <si>
     <t>RE-run the SAS program file from the previous step using the UI UAT version of SJM and observe the read-only attribute of the log and lst files</t>
+  </si>
+  <si>
+    <t>Line 1261</t>
   </si>
 </sst>
 </file>
@@ -2053,7 +2053,7 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -2088,7 +2088,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C3" s="64"/>
     </row>
@@ -2114,7 +2114,7 @@
         <v>78</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C6" s="69"/>
     </row>
@@ -2146,10 +2146,10 @@
         <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2177,10 +2177,10 @@
     </row>
     <row r="15" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="C15" s="10"/>
     </row>
@@ -2189,7 +2189,7 @@
         <v>89</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C16" s="10"/>
     </row>
@@ -2241,7 +2241,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -2267,7 +2267,7 @@
         <v>112</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="30" customFormat="1" ht="12" x14ac:dyDescent="0.25">
@@ -2388,50 +2388,50 @@
     </row>
     <row r="14" spans="1:5" s="30" customFormat="1" ht="84" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>110</v>
       </c>
       <c r="C14" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>189</v>
-      </c>
       <c r="E14" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="30" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B15" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="C15" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="D15" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="E15" s="30" t="s">
         <v>245</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="30" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>110</v>
       </c>
       <c r="C16" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>248</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="30" customFormat="1" ht="12" x14ac:dyDescent="0.25">
@@ -2538,7 +2538,7 @@
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2556,7 +2556,7 @@
         <v>174</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="71"/>
       <c r="E1" s="72"/>
@@ -2567,7 +2567,7 @@
         <v>175</v>
       </c>
       <c r="C2" s="70" t="s">
-        <v>177</v>
+        <v>263</v>
       </c>
       <c r="D2" s="71"/>
       <c r="E2" s="72"/>
@@ -2578,7 +2578,7 @@
         <v>176</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D3" s="71"/>
       <c r="E3" s="72"/>
@@ -2588,16 +2588,16 @@
         <v>103</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>173</v>
@@ -2608,7 +2608,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C5" s="61" t="s">
         <v>131</v>
@@ -2620,7 +2620,7 @@
         <v>159</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2628,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C6" s="61" t="s">
         <v>132</v>
@@ -2640,7 +2640,7 @@
         <v>160</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2648,7 +2648,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C7" s="61" t="s">
         <v>133</v>
@@ -2660,7 +2660,7 @@
         <v>161</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2668,7 +2668,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C8" s="61" t="s">
         <v>134</v>
@@ -2680,7 +2680,7 @@
         <v>162</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2688,7 +2688,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C9" s="61" t="s">
         <v>135</v>
@@ -2700,7 +2700,7 @@
         <v>163</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2708,19 +2708,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10" s="61" t="s">
         <v>136</v>
       </c>
       <c r="D10" s="61" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10" s="61" t="s">
         <v>164</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C11" s="61" t="s">
         <v>137</v>
@@ -2740,7 +2740,7 @@
         <v>165</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2748,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C12" s="61" t="s">
         <v>138</v>
@@ -2760,7 +2760,7 @@
         <v>166</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C13" s="61" t="s">
         <v>139</v>
@@ -2780,7 +2780,7 @@
         <v>167</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2788,19 +2788,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C14" s="61" t="s">
         <v>140</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E14" s="61" t="s">
         <v>168</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2808,7 +2808,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C15" s="61" t="s">
         <v>141</v>
@@ -2820,7 +2820,7 @@
         <v>169</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2828,19 +2828,19 @@
         <v>1</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C16" s="61" t="s">
         <v>142</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E16" s="61" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2848,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C17" s="61" t="s">
         <v>143</v>
@@ -2860,7 +2860,7 @@
         <v>170</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2868,7 +2868,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C18" s="61" t="s">
         <v>144</v>
@@ -2880,7 +2880,7 @@
         <v>171</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2888,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C19" s="61" t="s">
         <v>145</v>
@@ -2900,7 +2900,7 @@
         <v>172</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2908,19 +2908,19 @@
         <v>1</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C20" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="E20" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="E20" s="61" t="s">
-        <v>208</v>
-      </c>
       <c r="F20" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2928,19 +2928,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C21" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" s="61" t="s">
         <v>209</v>
       </c>
-      <c r="D21" s="61" t="s">
-        <v>210</v>
-      </c>
       <c r="E21" s="61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2948,19 +2948,19 @@
         <v>1</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C22" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="D22" s="61" t="s">
         <v>211</v>
       </c>
-      <c r="D22" s="61" t="s">
-        <v>212</v>
-      </c>
       <c r="E22" s="61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2968,19 +2968,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C23" s="61" t="s">
+        <v>212</v>
+      </c>
+      <c r="D23" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="D23" s="61" t="s">
-        <v>214</v>
-      </c>
       <c r="E23" s="61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2988,19 +2988,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C24" s="61" t="s">
+        <v>212</v>
+      </c>
+      <c r="D24" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="D24" s="61" t="s">
-        <v>214</v>
-      </c>
       <c r="E24" s="61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
@@ -3008,19 +3008,19 @@
         <v>2</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D25" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="E25" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="E25" s="61" t="s">
-        <v>191</v>
-      </c>
       <c r="F25" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -3028,19 +3028,19 @@
         <v>2</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C26" s="61" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="D26" s="61" t="s">
+      <c r="E26" s="61" t="s">
         <v>193</v>
       </c>
-      <c r="E26" s="61" t="s">
-        <v>194</v>
-      </c>
       <c r="F26" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -3048,19 +3048,19 @@
         <v>2</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C27" s="61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D27" s="61" t="s">
+        <v>192</v>
+      </c>
+      <c r="E27" s="61" t="s">
         <v>193</v>
       </c>
-      <c r="E27" s="61" t="s">
-        <v>194</v>
-      </c>
       <c r="F27" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -3068,19 +3068,19 @@
         <v>2</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C28" s="61" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="D28" s="61" t="s">
+      <c r="E28" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="E28" s="61" t="s">
-        <v>198</v>
-      </c>
       <c r="F28" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -3088,19 +3088,19 @@
         <v>3</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="D29" s="13" t="s">
+      <c r="E29" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>254</v>
-      </c>
       <c r="F29" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3189,9 +3189,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2:E2" r:id="rId1" display="Unit Tests" xr:uid="{D96ADB01-BA14-4E3C-B8EA-F456465AE71E}"/>
-    <hyperlink ref="C1:E1" r:id="rId2" display="Specifications" xr:uid="{871A1375-5E78-48D2-A4C8-C4E80B2F7A38}"/>
     <hyperlink ref="C3:E3" location="'Test Harness SS'!A1" display="Test Harness" xr:uid="{4E5465AB-A357-4422-A8C3-A1E628DB4AA5}"/>
+    <hyperlink ref="C2:E2" r:id="rId1" display="Line 1261" xr:uid="{B723BC6B-59BD-4737-A141-79C971203599}"/>
+    <hyperlink ref="C1:E1" r:id="rId2" display="Specifications" xr:uid="{81E48057-AA44-4E8C-BBD5-D88F4E3CB32F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="82" orientation="portrait" r:id="rId3"/>
@@ -3242,7 +3242,7 @@
         <v>174</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C1" s="71"/>
       <c r="D1" s="54"/>
@@ -3261,7 +3261,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>173</v>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="3" spans="1:6" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="59"/>
@@ -3369,10 +3369,10 @@
         <v>30</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.25">
@@ -3386,10 +3386,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.25">
@@ -3405,10 +3405,10 @@
       <c r="D5" s="42"/>
       <c r="E5" s="43"/>
       <c r="F5" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.25">
@@ -3422,10 +3422,10 @@
         <v>23</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3448,7 +3448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCC43BA-2873-4DC3-9BE6-B5E567C8252A}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3464,7 +3464,7 @@
         <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3472,7 +3472,7 @@
         <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -3500,10 +3500,10 @@
         <v>45400</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -3514,10 +3514,10 @@
         <v>45400</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>261</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>262</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -3527,10 +3527,10 @@
         <v>45400</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -3550,7 +3550,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -3600,7 +3600,7 @@
         <v>95</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" s="47">
         <v>45166</v>
@@ -3611,13 +3611,13 @@
         <v>25</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>185</v>
-      </c>
       <c r="D4" s="37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4" s="47">
         <v>45166</v>
@@ -3634,7 +3634,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E5" s="47">
         <v>45166</v>

</xml_diff>